<commit_message>
partly impl fundtransaction excel export, remain merge strategy to impl
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/investment-template.xlsx
+++ b/src/main/resources/templates/investment-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sichu\dev\investment-tool\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E80D707-6300-413E-93D0-1EDBE63AB497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3508E6-8D9F-4D6A-A309-9CD7F7371C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="63">
   <si>
     <t>编号</t>
   </si>
@@ -210,6 +210,12 @@
   </si>
   <si>
     <t>{.totalFee}</t>
+  </si>
+  <si>
+    <t>{.transactionDate}</t>
+  </si>
+  <si>
+    <t>交易所属日</t>
   </si>
 </sst>
 </file>
@@ -545,33 +551,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{033E134C-0186-423D-AFE4-35F8FA035D52}">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P16" sqref="P16"/>
+      <selection pane="bottomLeft" sqref="A1:S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" customWidth="1"/>
     <col min="2" max="2" width="44.28515625" customWidth="1"/>
-    <col min="3" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" customWidth="1"/>
-    <col min="11" max="12" width="9.42578125" customWidth="1"/>
-    <col min="13" max="13" width="9" customWidth="1"/>
-    <col min="14" max="14" width="11" customWidth="1"/>
-    <col min="15" max="15" width="11.7109375" customWidth="1"/>
-    <col min="16" max="16" width="80.28515625" customWidth="1"/>
-    <col min="17" max="17" width="29.42578125" customWidth="1"/>
-    <col min="18" max="18" width="17.28515625" customWidth="1"/>
+    <col min="3" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" customWidth="1"/>
+    <col min="12" max="13" width="9.42578125" customWidth="1"/>
+    <col min="14" max="14" width="9" customWidth="1"/>
+    <col min="15" max="15" width="11" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" customWidth="1"/>
+    <col min="18" max="18" width="80.28515625" customWidth="1"/>
+    <col min="19" max="19" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>57</v>
       </c>
@@ -592,8 +598,9 @@
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S1" s="4"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -604,52 +611,55 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -660,52 +670,55 @@
         <v>24</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="R3" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -724,8 +737,9 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S4" s="2"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -744,8 +758,9 @@
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S5" s="2"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -764,10 +779,11 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -779,7 +795,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,8 +806,8 @@
     <col min="6" max="6" width="11.140625" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
     <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.42578125" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -834,10 +850,10 @@
         <v>11</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -866,10 +882,10 @@
         <v>47</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
partly impl Fund Transaction Report Sheet export, TODO: solve heldDays and redemption wrong data
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/investment-template.xlsx
+++ b/src/main/resources/templates/investment-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sichu\dev\investment-tool\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3508E6-8D9F-4D6A-A309-9CD7F7371C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00A9D56-4628-41F6-84E0-3377AC832E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="65">
   <si>
     <t>编号</t>
   </si>
@@ -86,9 +86,6 @@
     <t>{.totalAmount}</t>
   </si>
   <si>
-    <t>{.heldDate}</t>
-  </si>
-  <si>
     <t>净收益</t>
   </si>
   <si>
@@ -179,21 +176,6 @@
     <t>{.totalShare}</t>
   </si>
   <si>
-    <t>购买交易申请日</t>
-  </si>
-  <si>
-    <t>{.purchaseApplicationDate}</t>
-  </si>
-  <si>
-    <t>赎回交易申请日</t>
-  </si>
-  <si>
-    <t>{.redemptionApplicationDate}</t>
-  </si>
-  <si>
-    <t>分红交易日</t>
-  </si>
-  <si>
     <t>{.dividendDate}</t>
   </si>
   <si>
@@ -216,6 +198,30 @@
   </si>
   <si>
     <t>交易所属日</t>
+  </si>
+  <si>
+    <t>购买交易所属日</t>
+  </si>
+  <si>
+    <t>赎回交易所属日</t>
+  </si>
+  <si>
+    <t>分红交易所属日</t>
+  </si>
+  <si>
+    <t>{.purchaseTransactionDate}</t>
+  </si>
+  <si>
+    <t>{.redemptionTransactionDate}</t>
+  </si>
+  <si>
+    <t>{.heldDays}</t>
+  </si>
+  <si>
+    <t>合计本金</t>
+  </si>
+  <si>
+    <t>{.totalPrincipalAmount}</t>
   </si>
 </sst>
 </file>
@@ -579,7 +585,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -611,25 +617,25 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>4</v>
@@ -647,7 +653,7 @@
         <v>8</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>13</v>
@@ -667,55 +673,55 @@
         <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="G3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="M3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>18</v>
       </c>
       <c r="P3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S3" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -792,10 +798,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7092094F-6C7F-4772-8365-89902B97E981}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,15 +810,15 @@
     <col min="2" max="2" width="44.28515625" customWidth="1"/>
     <col min="3" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.42578125" customWidth="1"/>
+    <col min="7" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -823,8 +829,10 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -832,31 +840,37 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -864,35 +878,42 @@
         <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>34</v>
+        <v>46</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -922,7 +943,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -938,37 +959,37 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>13</v>
@@ -976,40 +997,40 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upgrade to v1.0.1, solve some bugs, wait to fix excel report template relevant bugs
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/investment-template.xlsx
+++ b/src/main/resources/templates/investment-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sichu\dev\investment-tool\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00A9D56-4628-41F6-84E0-3377AC832E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA67D963-16BE-43C5-89D2-FB42941827D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="67">
   <si>
     <t>编号</t>
   </si>
@@ -222,6 +222,12 @@
   </si>
   <si>
     <t>{.totalPrincipalAmount}</t>
+  </si>
+  <si>
+    <t>现金分红</t>
+  </si>
+  <si>
+    <t>{.dividendAmountPerShare}</t>
   </si>
 </sst>
 </file>
@@ -557,11 +563,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{033E134C-0186-423D-AFE4-35F8FA035D52}">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:S1"/>
+      <selection pane="bottomLeft" sqref="A1:T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,16 +580,16 @@
     <col min="9" max="9" width="10.28515625" customWidth="1"/>
     <col min="10" max="10" width="11.140625" customWidth="1"/>
     <col min="11" max="11" width="7.7109375" customWidth="1"/>
-    <col min="12" max="13" width="9.42578125" customWidth="1"/>
-    <col min="14" max="14" width="9" customWidth="1"/>
-    <col min="15" max="15" width="11" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" customWidth="1"/>
-    <col min="17" max="17" width="16.7109375" customWidth="1"/>
-    <col min="18" max="18" width="80.28515625" customWidth="1"/>
-    <col min="19" max="19" width="29.42578125" customWidth="1"/>
+    <col min="12" max="14" width="9.42578125" customWidth="1"/>
+    <col min="15" max="15" width="9" customWidth="1"/>
+    <col min="16" max="16" width="11" customWidth="1"/>
+    <col min="17" max="17" width="11.7109375" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" customWidth="1"/>
+    <col min="19" max="19" width="80.28515625" customWidth="1"/>
+    <col min="20" max="20" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>51</v>
       </c>
@@ -605,8 +611,9 @@
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
       <c r="S1" s="4"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" s="4"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -646,26 +653,29 @@
       <c r="M2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -705,26 +715,29 @@
       <c r="M3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="N3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="O3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -744,8 +757,9 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T4" s="2"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -765,8 +779,9 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T5" s="2"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -786,10 +801,11 @@
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A1:T1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update to v1.1.0 with only limited tests, seperate dev/prod environment, simplify codes and fix bugs and update tables and columns
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/investment-template.xlsx
+++ b/src/main/resources/templates/investment-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sichu\dev\investment-tool\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA67D963-16BE-43C5-89D2-FB42941827D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714FACCD-81CE-4E38-816A-E6A810B64C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="71">
   <si>
     <t>编号</t>
   </si>
@@ -176,9 +176,6 @@
     <t>{.totalShare}</t>
   </si>
   <si>
-    <t>{.dividendDate}</t>
-  </si>
-  <si>
     <t>Fund Transaction Report</t>
   </si>
   <si>
@@ -206,9 +203,6 @@
     <t>赎回交易所属日</t>
   </si>
   <si>
-    <t>分红交易所属日</t>
-  </si>
-  <si>
     <t>{.purchaseTransactionDate}</t>
   </si>
   <si>
@@ -228,6 +222,24 @@
   </si>
   <si>
     <t>{.dividendAmountPerShare}</t>
+  </si>
+  <si>
+    <t>分红次数</t>
+  </si>
+  <si>
+    <t>{.dividendCount}</t>
+  </si>
+  <si>
+    <t>收益率</t>
+  </si>
+  <si>
+    <t>{.yieldRate}</t>
+  </si>
+  <si>
+    <t>{.totalDividendAmount}</t>
+  </si>
+  <si>
+    <t>合计分红金额</t>
   </si>
 </sst>
 </file>
@@ -591,7 +603,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -624,7 +636,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>24</v>
@@ -636,7 +648,7 @@
         <v>9</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>3</v>
@@ -654,7 +666,7 @@
         <v>6</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>7</v>
@@ -686,7 +698,7 @@
         <v>23</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>34</v>
@@ -698,7 +710,7 @@
         <v>26</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>27</v>
@@ -716,7 +728,7 @@
         <v>29</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>30</v>
@@ -814,27 +826,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7092094F-6C7F-4772-8365-89902B97E981}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+      <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" customWidth="1"/>
     <col min="2" max="2" width="44.28515625" customWidth="1"/>
-    <col min="3" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" customWidth="1"/>
-    <col min="7" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.42578125" customWidth="1"/>
+    <col min="3" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -847,8 +861,10 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -856,37 +872,43 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -894,39 +916,45 @@
         <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>62</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>64</v>
+        <v>18</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -959,7 +987,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>

</xml_diff>

<commit_message>
delete useless/redundant service & mapper, optimize excel template export service
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/investment-template.xlsx
+++ b/src/main/resources/templates/investment-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sichu\dev\investment-tool\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D899DA-7EDF-428F-AEF0-A498DD49E992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB94DAC-4F74-4387-9AB6-9B8D235FB2BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="83">
   <si>
     <t>编号</t>
   </si>
@@ -267,12 +267,6 @@
   </si>
   <si>
     <t>平均收益率</t>
-  </si>
-  <si>
-    <t>平均日均万份收益</t>
-  </si>
-  <si>
-    <t>{avgDailyNavYield}</t>
   </si>
   <si>
     <t>{avgYieldRate}</t>
@@ -881,9 +875,8 @@
     <col min="3" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="7" width="11" customWidth="1"/>
     <col min="8" max="9" width="13.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" customWidth="1"/>
-    <col min="12" max="12" width="11" customWidth="1"/>
+    <col min="10" max="11" width="11" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" customWidth="1"/>
     <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="29.42578125" customWidth="1"/>
   </cols>
@@ -938,10 +931,10 @@
         <v>19</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>13</v>
@@ -982,10 +975,10 @@
         <v>20</v>
       </c>
       <c r="K3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>22</v>
@@ -1023,7 +1016,7 @@
         <v>73</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>75</v>
@@ -1032,11 +1025,9 @@
         <v>77</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="L5" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
@@ -1053,7 +1044,7 @@
         <v>74</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>76</v>
@@ -1062,11 +1053,9 @@
         <v>78</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>82</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>

</xml_diff>

<commit_message>
v1.2.0, integrate duplicated calculation code to methods, change new excel template for quicker and better analysis, change entities' toString methods to apache common lang3 for quicker toString
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/investment-template.xlsx
+++ b/src/main/resources/templates/investment-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sichu\dev\investment-tool\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB94DAC-4F74-4387-9AB6-9B8D235FB2BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD9C0D0-137D-4432-ABF1-E59F32BC58AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -266,16 +266,16 @@
     <t>{sumProfit}</t>
   </si>
   <si>
-    <t>平均收益率</t>
-  </si>
-  <si>
-    <t>{avgYieldRate}</t>
-  </si>
-  <si>
     <t>累计分红次数</t>
   </si>
   <si>
     <t>{sumDividendCount}</t>
+  </si>
+  <si>
+    <t>累计收益率</t>
+  </si>
+  <si>
+    <t>{totalYieldRate}</t>
   </si>
 </sst>
 </file>
@@ -621,20 +621,19 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="44.28515625" customWidth="1"/>
-    <col min="3" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" customWidth="1"/>
+    <col min="2" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="9" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
     <col min="9" max="9" width="10.28515625" customWidth="1"/>
     <col min="10" max="10" width="11.140625" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" customWidth="1"/>
-    <col min="12" max="14" width="9.42578125" customWidth="1"/>
-    <col min="15" max="15" width="9" customWidth="1"/>
-    <col min="16" max="16" width="11" customWidth="1"/>
-    <col min="17" max="17" width="11.7109375" customWidth="1"/>
-    <col min="18" max="18" width="16.7109375" customWidth="1"/>
-    <col min="19" max="19" width="80.28515625" customWidth="1"/>
-    <col min="20" max="20" width="29.42578125" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" customWidth="1"/>
+    <col min="12" max="12" width="7.28515625" customWidth="1"/>
+    <col min="13" max="13" width="11" customWidth="1"/>
+    <col min="14" max="14" width="7.7109375" customWidth="1"/>
+    <col min="15" max="17" width="9.42578125" customWidth="1"/>
+    <col min="18" max="18" width="44.28515625" customWidth="1"/>
+    <col min="19" max="19" width="29.42578125" customWidth="1"/>
+    <col min="20" max="20" width="80.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -666,7 +665,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
@@ -681,10 +680,10 @@
         <v>25</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>52</v>
+        <v>7</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>3</v>
@@ -693,34 +692,34 @@
         <v>47</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="R2" s="2" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="S2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="T2" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -728,7 +727,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>23</v>
@@ -743,10 +742,10 @@
         <v>35</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>53</v>
+        <v>30</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>27</v>
@@ -755,34 +754,34 @@
         <v>48</v>
       </c>
       <c r="K3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="R3" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="S3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="T3" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -1016,7 +1015,7 @@
         <v>73</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>75</v>
@@ -1025,7 +1024,7 @@
         <v>77</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -1044,7 +1043,7 @@
         <v>74</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>76</v>
@@ -1053,7 +1052,7 @@
         <v>78</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>

</xml_diff>

<commit_message>
add gold transaction entity, excel, mapper, todo: gold sheet mapper & gold transaction controller
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/investment-template.xlsx
+++ b/src/main/resources/templates/investment-template.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sichu\dev\investment-tool\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD9C0D0-137D-4432-ABF1-E59F32BC58AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC57C1BD-B2E7-41F6-AA3C-9F2735EAD9AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fund Transaction Statement" sheetId="5" r:id="rId1"/>
     <sheet name="Fund Transaction Report" sheetId="3" r:id="rId2"/>
-    <sheet name="Gold Transaction Statement" sheetId="4" r:id="rId3"/>
+    <sheet name="Gold Transaction Summary" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="88">
   <si>
     <t>编号</t>
   </si>
@@ -137,15 +137,6 @@
     <t>{.settlementDate}</t>
   </si>
   <si>
-    <t>名称</t>
-  </si>
-  <si>
-    <t>{.name}</t>
-  </si>
-  <si>
-    <t>{.amountPerGram}</t>
-  </si>
-  <si>
     <t>交易金额/克</t>
   </si>
   <si>
@@ -155,18 +146,6 @@
     <t>{.grams}</t>
   </si>
   <si>
-    <t>合计克数</t>
-  </si>
-  <si>
-    <t>平均交易金额/克</t>
-  </si>
-  <si>
-    <t>{.avgAmountPerGram}</t>
-  </si>
-  <si>
-    <t>{.totalGrams}</t>
-  </si>
-  <si>
     <t>{.dailyNavYield}</t>
   </si>
   <si>
@@ -276,6 +255,42 @@
   </si>
   <si>
     <t>{totalYieldRate}</t>
+  </si>
+  <si>
+    <t>{.pircePerGram}</t>
+  </si>
+  <si>
+    <t>{.purchaseTime}</t>
+  </si>
+  <si>
+    <t>{.redemptionTime}</t>
+  </si>
+  <si>
+    <t>累计克数</t>
+  </si>
+  <si>
+    <t>{sumPrincipalAmount}</t>
+  </si>
+  <si>
+    <t>{sumAmount}</t>
+  </si>
+  <si>
+    <t>{sumYieldRate}</t>
+  </si>
+  <si>
+    <t>{sumGrams}</t>
+  </si>
+  <si>
+    <t>平均金额/克</t>
+  </si>
+  <si>
+    <t>购买时间</t>
+  </si>
+  <si>
+    <t>赎回时间</t>
+  </si>
+  <si>
+    <t>{avgAmountPerGram}</t>
   </si>
 </sst>
 </file>
@@ -317,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -330,6 +345,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -613,7 +631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{033E134C-0186-423D-AFE4-35F8FA035D52}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:T1"/>
     </sheetView>
@@ -638,7 +656,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -671,7 +689,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>24</v>
@@ -689,7 +707,7 @@
         <v>3</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>13</v>
@@ -698,7 +716,7 @@
         <v>9</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>4</v>
@@ -710,7 +728,7 @@
         <v>6</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>1</v>
@@ -733,7 +751,7 @@
         <v>23</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>34</v>
@@ -751,7 +769,7 @@
         <v>27</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>22</v>
@@ -760,7 +778,7 @@
         <v>26</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>28</v>
@@ -772,7 +790,7 @@
         <v>29</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="R3" s="2" t="s">
         <v>15</v>
@@ -882,7 +900,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -906,31 +924,31 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>11</v>
@@ -950,34 +968,34 @@
         <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>22</v>
@@ -1009,22 +1027,22 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -1037,22 +1055,22 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -1133,31 +1151,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE0EEB1-C90D-4F9C-9602-284D8CA8FAFF}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="10" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1165,91 +1172,195 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>37</v>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>22</v>
       </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add gold excel export impl, todo: gold controller and test
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/investment-template.xlsx
+++ b/src/main/resources/templates/investment-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sichu\dev\investment-tool\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC57C1BD-B2E7-41F6-AA3C-9F2735EAD9AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0380689B-D6EF-447F-AF81-D7DFE3E6DA42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -344,10 +344,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -655,28 +655,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -899,22 +899,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1163,18 +1163,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">

</xml_diff>

<commit_message>
v1.2.2, impl gold controller, and pass test, TODO: solve gold position bug
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/investment-template.xlsx
+++ b/src/main/resources/templates/investment-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sichu\dev\investment-tool\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0380689B-D6EF-447F-AF81-D7DFE3E6DA42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488E629D-0787-48AC-A583-650A3C527410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="930" windowWidth="19110" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fund Transaction Statement" sheetId="5" r:id="rId1"/>
@@ -631,7 +631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{033E134C-0186-423D-AFE4-35F8FA035D52}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:T1"/>
     </sheetView>
@@ -1153,7 +1153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE0EEB1-C90D-4F9C-9602-284D8CA8FAFF}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>

</xml_diff>